<commit_message>
Estructuras y verificación de los dígitos de control
</commit_message>
<xml_diff>
--- a/src/resources/SistemasInformacionII.xlsx
+++ b/src/resources/SistemasInformacionII.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="532">
   <si>
     <t>Nombre</t>
   </si>
@@ -1487,6 +1487,144 @@
   </si>
   <si>
     <t>09611071S</t>
+  </si>
+  <si>
+    <t>209600431143554600000</t>
+  </si>
+  <si>
+    <t>321454641038452163421</t>
+  </si>
+  <si>
+    <t>325695231116220165156</t>
+  </si>
+  <si>
+    <t>201250033115201112544</t>
+  </si>
+  <si>
+    <t>232154653105456411515</t>
+  </si>
+  <si>
+    <t>215849769112154655487</t>
+  </si>
+  <si>
+    <t>9643124510108150005156</t>
+  </si>
+  <si>
+    <t>250300001014574745458</t>
+  </si>
+  <si>
+    <t>159536848101254695203</t>
+  </si>
+  <si>
+    <t>209600431123096200000</t>
+  </si>
+  <si>
+    <t>209600431132159000000</t>
+  </si>
+  <si>
+    <t>126696811105112121210</t>
+  </si>
+  <si>
+    <t>255168481121156151054</t>
+  </si>
+  <si>
+    <t>666494441062310000255</t>
+  </si>
+  <si>
+    <t>362500128114785523365</t>
+  </si>
+  <si>
+    <t>225156519105640081000</t>
+  </si>
+  <si>
+    <t>213461545113164978451</t>
+  </si>
+  <si>
+    <t>245879461132003165464</t>
+  </si>
+  <si>
+    <t>209600431173071400000</t>
+  </si>
+  <si>
+    <t>209600431142158800000</t>
+  </si>
+  <si>
+    <t>665522111048855332200</t>
+  </si>
+  <si>
+    <t>209600431143075700000</t>
+  </si>
+  <si>
+    <t>516514879100005118185</t>
+  </si>
+  <si>
+    <t>018265301020201560000</t>
+  </si>
+  <si>
+    <t>209600431133000100000</t>
+  </si>
+  <si>
+    <t>316245611142546920007</t>
+  </si>
+  <si>
+    <t>361542317102500312566</t>
+  </si>
+  <si>
+    <t>448756641027231645789</t>
+  </si>
+  <si>
+    <t>625815427103690044508</t>
+  </si>
+  <si>
+    <t>369523651120014425254</t>
+  </si>
+  <si>
+    <t>214163258101510005514</t>
+  </si>
+  <si>
+    <t>326284845114115151115</t>
+  </si>
+  <si>
+    <t>20960056133231500000</t>
+  </si>
+  <si>
+    <t>23658965274585223202</t>
+  </si>
+  <si>
+    <t>236523651042254222000</t>
+  </si>
+  <si>
+    <t>200125411050023365233</t>
+  </si>
+  <si>
+    <t>362459781033245679001</t>
+  </si>
+  <si>
+    <t>325745121185411002255</t>
+  </si>
+  <si>
+    <t>2096004311103468900000</t>
+  </si>
+  <si>
+    <t>651656549108886005001</t>
+  </si>
+  <si>
+    <t>51556584221251000254</t>
+  </si>
+  <si>
+    <t>62541122421110105611</t>
+  </si>
+  <si>
+    <t>65645150865168448896</t>
+  </si>
+  <si>
+    <t>265516818117651415636</t>
+  </si>
+  <si>
+    <t>111122235114444444444</t>
+  </si>
+  <si>
+    <t>11112223504444444444</t>
   </si>
 </sst>
 </file>
@@ -1985,7 +2123,7 @@
         <v>70</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>80</v>
+        <v>531</v>
       </c>
       <c r="K2" t="s">
         <v>85</v>
@@ -2021,7 +2159,7 @@
         <v>70</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>388</v>
+        <v>531</v>
       </c>
       <c r="K3" t="s">
         <v>85</v>
@@ -2057,7 +2195,7 @@
         <v>133</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>389</v>
+        <v>531</v>
       </c>
       <c r="K4" t="s">
         <v>90</v>
@@ -2093,7 +2231,7 @@
         <v>485</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>390</v>
+        <v>531</v>
       </c>
       <c r="K5" t="s">
         <v>85</v>
@@ -2129,7 +2267,7 @@
         <v>238</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>391</v>
+        <v>531</v>
       </c>
       <c r="K6" t="s">
         <v>374</v>
@@ -2165,7 +2303,7 @@
         <v>355</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>392</v>
+        <v>531</v>
       </c>
       <c r="K7" t="s">
         <v>86</v>
@@ -2201,7 +2339,7 @@
         <v>250</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>393</v>
+        <v>531</v>
       </c>
       <c r="K8" t="s">
         <v>367</v>
@@ -2241,7 +2379,7 @@
         <v>168</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>394</v>
+        <v>531</v>
       </c>
       <c r="K10" t="s">
         <v>87</v>
@@ -2277,7 +2415,7 @@
         <v>279</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>395</v>
+        <v>531</v>
       </c>
       <c r="K11" t="s">
         <v>85</v>
@@ -2313,7 +2451,7 @@
         <v>396</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>80</v>
+        <v>531</v>
       </c>
       <c r="K12" t="s">
         <v>89</v>
@@ -2349,7 +2487,7 @@
         <v>396</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>397</v>
+        <v>531</v>
       </c>
       <c r="K13" t="s">
         <v>85</v>
@@ -2385,7 +2523,7 @@
         <v>286</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>398</v>
+        <v>531</v>
       </c>
       <c r="K14" t="s">
         <v>371</v>
@@ -2421,7 +2559,7 @@
         <v>267</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>399</v>
+        <v>531</v>
       </c>
       <c r="K15" t="s">
         <v>377</v>
@@ -2454,7 +2592,7 @@
         <v>359</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>400</v>
+        <v>531</v>
       </c>
       <c r="K16" t="s">
         <v>88</v>
@@ -2490,7 +2628,7 @@
         <v>359</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>401</v>
+        <v>531</v>
       </c>
       <c r="K17" t="s">
         <v>85</v>
@@ -2526,7 +2664,7 @@
         <v>330</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>402</v>
+        <v>531</v>
       </c>
       <c r="K18" t="s">
         <v>376</v>
@@ -2562,7 +2700,7 @@
         <v>317</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>403</v>
+        <v>531</v>
       </c>
       <c r="K19" t="s">
         <v>85</v>
@@ -2598,7 +2736,7 @@
         <v>327</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>404</v>
+        <v>531</v>
       </c>
       <c r="K20" t="s">
         <v>368</v>
@@ -2634,7 +2772,7 @@
         <v>313</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>405</v>
+        <v>531</v>
       </c>
       <c r="K21" t="s">
         <v>370</v>
@@ -2670,7 +2808,7 @@
         <v>43</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>406</v>
+        <v>531</v>
       </c>
       <c r="K22" t="s">
         <v>85</v>
@@ -2703,7 +2841,7 @@
         <v>407</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>400</v>
+        <v>531</v>
       </c>
       <c r="K23" t="s">
         <v>90</v>
@@ -2739,7 +2877,7 @@
         <v>407</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>408</v>
+        <v>531</v>
       </c>
       <c r="K24" t="s">
         <v>85</v>
@@ -2772,7 +2910,7 @@
         <v>64</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>81</v>
+        <v>531</v>
       </c>
       <c r="K25" t="s">
         <v>87</v>
@@ -2808,7 +2946,7 @@
         <v>409</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>410</v>
+        <v>531</v>
       </c>
       <c r="K26" t="s">
         <v>85</v>
@@ -2844,7 +2982,7 @@
         <v>198</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>411</v>
+        <v>531</v>
       </c>
       <c r="K27" t="s">
         <v>86</v>
@@ -2884,7 +3022,7 @@
         <v>300</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>412</v>
+        <v>531</v>
       </c>
       <c r="K29" t="s">
         <v>85</v>
@@ -2920,7 +3058,7 @@
         <v>186</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>413</v>
+        <v>531</v>
       </c>
       <c r="K30" t="s">
         <v>85</v>
@@ -2956,7 +3094,7 @@
         <v>321</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>414</v>
+        <v>531</v>
       </c>
       <c r="K31" t="s">
         <v>380</v>
@@ -2992,7 +3130,7 @@
         <v>325</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>415</v>
+        <v>531</v>
       </c>
       <c r="K32" t="s">
         <v>85</v>
@@ -3028,7 +3166,7 @@
         <v>334</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>416</v>
+        <v>531</v>
       </c>
       <c r="K33" t="s">
         <v>85</v>
@@ -3064,7 +3202,7 @@
         <v>270</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>417</v>
+        <v>531</v>
       </c>
       <c r="K34" t="s">
         <v>378</v>
@@ -3100,7 +3238,7 @@
         <v>217</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>418</v>
+        <v>531</v>
       </c>
       <c r="K35" t="s">
         <v>85</v>
@@ -3136,7 +3274,7 @@
         <v>235</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>419</v>
+        <v>531</v>
       </c>
       <c r="K36" t="s">
         <v>373</v>
@@ -3172,7 +3310,7 @@
         <v>210</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>420</v>
+        <v>531</v>
       </c>
       <c r="K37" t="s">
         <v>368</v>
@@ -3208,7 +3346,7 @@
         <v>350</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>421</v>
+        <v>531</v>
       </c>
       <c r="K38" t="s">
         <v>86</v>
@@ -3244,7 +3382,7 @@
         <v>422</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>423</v>
+        <v>531</v>
       </c>
       <c r="K39" t="s">
         <v>86</v>
@@ -3280,7 +3418,7 @@
         <v>337</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>424</v>
+        <v>531</v>
       </c>
       <c r="K40" t="s">
         <v>85</v>
@@ -3316,7 +3454,7 @@
         <v>341</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>425</v>
+        <v>531</v>
       </c>
       <c r="K41" t="s">
         <v>85</v>
@@ -3352,7 +3490,7 @@
         <v>126</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>426</v>
+        <v>531</v>
       </c>
       <c r="K42" t="s">
         <v>85</v>
@@ -3388,7 +3526,7 @@
         <v>344</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>427</v>
+        <v>531</v>
       </c>
       <c r="K43" t="s">
         <v>85</v>
@@ -3424,7 +3562,7 @@
         <v>348</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>428</v>
+        <v>531</v>
       </c>
       <c r="K44" t="s">
         <v>89</v>
@@ -3460,7 +3598,7 @@
         <v>429</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>430</v>
+        <v>531</v>
       </c>
       <c r="K45" t="s">
         <v>85</v>
@@ -3496,7 +3634,7 @@
         <v>42</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>431</v>
+        <v>531</v>
       </c>
       <c r="K46" t="s">
         <v>85</v>
@@ -3532,7 +3670,7 @@
         <v>182</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>432</v>
+        <v>531</v>
       </c>
       <c r="K47" t="s">
         <v>85</v>
@@ -3568,7 +3706,7 @@
         <v>141</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>433</v>
+        <v>531</v>
       </c>
       <c r="K48" t="s">
         <v>85</v>
@@ -3604,7 +3742,7 @@
         <v>246</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>434</v>
+        <v>531</v>
       </c>
       <c r="K49" t="s">
         <v>85</v>
@@ -3637,7 +3775,7 @@
         <v>435</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>81</v>
+        <v>531</v>
       </c>
       <c r="K50" t="s">
         <v>91</v>
@@ -3670,7 +3808,7 @@
         <v>436</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>437</v>
+        <v>531</v>
       </c>
       <c r="K51" t="s">
         <v>86</v>
@@ -3706,7 +3844,7 @@
         <v>137</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>438</v>
+        <v>531</v>
       </c>
       <c r="K52" t="s">
         <v>86</v>
@@ -3742,7 +3880,7 @@
         <v>439</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>440</v>
+        <v>531</v>
       </c>
       <c r="K53" t="s">
         <v>85</v>
@@ -3778,7 +3916,7 @@
         <v>248</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>441</v>
+        <v>531</v>
       </c>
       <c r="K54" t="s">
         <v>376</v>
@@ -3814,7 +3952,7 @@
         <v>192</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>442</v>
+        <v>531</v>
       </c>
       <c r="K55" t="s">
         <v>85</v>
@@ -3850,7 +3988,7 @@
         <v>207</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>443</v>
+        <v>531</v>
       </c>
       <c r="K56" t="s">
         <v>87</v>
@@ -3886,7 +4024,7 @@
         <v>170</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>444</v>
+        <v>531</v>
       </c>
       <c r="K57" t="s">
         <v>91</v>
@@ -3922,7 +4060,7 @@
         <v>277</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>445</v>
+        <v>531</v>
       </c>
       <c r="K58" t="s">
         <v>85</v>
@@ -3962,7 +4100,7 @@
         <v>446</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>79</v>
+        <v>531</v>
       </c>
       <c r="K60" t="s">
         <v>85</v>
@@ -3998,7 +4136,7 @@
         <v>194</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>447</v>
+        <v>531</v>
       </c>
       <c r="K61" t="s">
         <v>85</v>
@@ -4034,7 +4172,7 @@
         <v>69</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>448</v>
+        <v>531</v>
       </c>
       <c r="K62" t="s">
         <v>85</v>
@@ -4070,7 +4208,7 @@
         <v>204</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>449</v>
+        <v>531</v>
       </c>
       <c r="K63" t="s">
         <v>91</v>
@@ -4106,7 +4244,7 @@
         <v>122</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>450</v>
+        <v>531</v>
       </c>
       <c r="K64" t="s">
         <v>85</v>
@@ -4142,7 +4280,7 @@
         <v>221</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>451</v>
+        <v>531</v>
       </c>
       <c r="K65" t="s">
         <v>85</v>
@@ -4178,7 +4316,7 @@
         <v>152</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>452</v>
+        <v>531</v>
       </c>
       <c r="K66" t="s">
         <v>85</v>
@@ -4214,7 +4352,7 @@
         <v>358</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>453</v>
+        <v>531</v>
       </c>
       <c r="K67" t="s">
         <v>85</v>
@@ -4250,7 +4388,7 @@
         <v>435</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>77</v>
+        <v>531</v>
       </c>
       <c r="K68" t="s">
         <v>85</v>
@@ -4286,7 +4424,7 @@
         <v>454</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>455</v>
+        <v>531</v>
       </c>
       <c r="K69" t="s">
         <v>85</v>
@@ -4322,7 +4460,7 @@
         <v>252</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>456</v>
+        <v>531</v>
       </c>
       <c r="K70" t="s">
         <v>85</v>
@@ -4358,7 +4496,7 @@
         <v>164</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>457</v>
+        <v>531</v>
       </c>
       <c r="K71" t="s">
         <v>85</v>
@@ -4394,7 +4532,7 @@
         <v>283</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>458</v>
+        <v>531</v>
       </c>
       <c r="K72" t="s">
         <v>85</v>
@@ -4430,7 +4568,7 @@
         <v>422</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>448</v>
+        <v>531</v>
       </c>
       <c r="K73" t="s">
         <v>85</v>
@@ -4466,7 +4604,7 @@
         <v>304</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>459</v>
+        <v>531</v>
       </c>
       <c r="K74" t="s">
         <v>380</v>
@@ -4502,7 +4640,7 @@
         <v>297</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>460</v>
+        <v>531</v>
       </c>
       <c r="K75" t="s">
         <v>85</v>
@@ -4538,7 +4676,7 @@
         <v>69</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>461</v>
+        <v>531</v>
       </c>
       <c r="K76" t="s">
         <v>85</v>
@@ -4574,7 +4712,7 @@
         <v>254</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>462</v>
+        <v>531</v>
       </c>
       <c r="K77" t="s">
         <v>85</v>
@@ -4610,7 +4748,7 @@
         <v>232</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>463</v>
+        <v>531</v>
       </c>
       <c r="K78" t="s">
         <v>372</v>
@@ -4648,7 +4786,7 @@
       </c>
       <c r="H80" s="3"/>
       <c r="J80" s="5" t="s">
-        <v>78</v>
+        <v>531</v>
       </c>
       <c r="K80" t="s">
         <v>85</v>
@@ -4683,7 +4821,7 @@
         <v>174</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>464</v>
+        <v>531</v>
       </c>
       <c r="K81" t="s">
         <v>85</v>
@@ -4719,7 +4857,7 @@
         <v>310</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>366</v>
+        <v>531</v>
       </c>
       <c r="K82" t="s">
         <v>85</v>
@@ -4754,7 +4892,7 @@
         <v>130</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>465</v>
+        <v>531</v>
       </c>
       <c r="K83" t="s">
         <v>89</v>
@@ -4790,7 +4928,7 @@
         <v>294</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>466</v>
+        <v>531</v>
       </c>
       <c r="K84" t="s">
         <v>85</v>
@@ -4823,7 +4961,7 @@
         <v>291</v>
       </c>
       <c r="J85" s="5" t="s">
-        <v>365</v>
+        <v>531</v>
       </c>
       <c r="K85" t="s">
         <v>378</v>
@@ -4858,7 +4996,7 @@
         <v>256</v>
       </c>
       <c r="J86" s="5" t="s">
-        <v>467</v>
+        <v>531</v>
       </c>
       <c r="K86" t="s">
         <v>85</v>
@@ -4894,7 +5032,7 @@
         <v>145</v>
       </c>
       <c r="J87" s="5" t="s">
-        <v>468</v>
+        <v>531</v>
       </c>
       <c r="K87" t="s">
         <v>85</v>
@@ -4930,7 +5068,7 @@
         <v>148</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>469</v>
+        <v>531</v>
       </c>
       <c r="K88" t="s">
         <v>85</v>
@@ -4966,7 +5104,7 @@
         <v>259</v>
       </c>
       <c r="J89" s="5" t="s">
-        <v>470</v>
+        <v>531</v>
       </c>
       <c r="K89" t="s">
         <v>371</v>
@@ -5002,7 +5140,7 @@
         <v>156</v>
       </c>
       <c r="J90" s="5" t="s">
-        <v>471</v>
+        <v>531</v>
       </c>
       <c r="K90" t="s">
         <v>85</v>
@@ -5038,7 +5176,7 @@
         <v>118</v>
       </c>
       <c r="J91" s="5" t="s">
-        <v>472</v>
+        <v>531</v>
       </c>
       <c r="K91" t="s">
         <v>85</v>
@@ -5074,7 +5212,7 @@
         <v>288</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>473</v>
+        <v>531</v>
       </c>
       <c r="K92" t="s">
         <v>376</v>
@@ -5110,7 +5248,7 @@
         <v>242</v>
       </c>
       <c r="J93" s="5" t="s">
-        <v>474</v>
+        <v>531</v>
       </c>
       <c r="K93" t="s">
         <v>375</v>
@@ -5146,7 +5284,7 @@
         <v>44</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>475</v>
+        <v>531</v>
       </c>
       <c r="K94" t="s">
         <v>85</v>
@@ -5182,7 +5320,7 @@
         <v>476</v>
       </c>
       <c r="J95" s="5" t="s">
-        <v>477</v>
+        <v>531</v>
       </c>
       <c r="K95" t="s">
         <v>85</v>
@@ -5218,7 +5356,7 @@
         <v>478</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>479</v>
+        <v>531</v>
       </c>
       <c r="K96" t="s">
         <v>368</v>
@@ -5254,7 +5392,7 @@
         <v>178</v>
       </c>
       <c r="J97" s="5" t="s">
-        <v>480</v>
+        <v>531</v>
       </c>
       <c r="K97" t="s">
         <v>85</v>
@@ -5290,7 +5428,7 @@
         <v>160</v>
       </c>
       <c r="J98" s="5" t="s">
-        <v>481</v>
+        <v>531</v>
       </c>
       <c r="K98" t="s">
         <v>85</v>
@@ -5326,7 +5464,7 @@
         <v>115</v>
       </c>
       <c r="J99" s="5" t="s">
-        <v>482</v>
+        <v>531</v>
       </c>
       <c r="K99" t="s">
         <v>85</v>
@@ -5366,7 +5504,7 @@
         <v>213</v>
       </c>
       <c r="J101" s="5" t="s">
-        <v>361</v>
+        <v>531</v>
       </c>
       <c r="K101" t="s">
         <v>369</v>
@@ -5401,7 +5539,7 @@
         <v>201</v>
       </c>
       <c r="J102" s="5" t="s">
-        <v>483</v>
+        <v>531</v>
       </c>
       <c r="K102" t="s">
         <v>90</v>
@@ -5437,7 +5575,7 @@
         <v>228</v>
       </c>
       <c r="J103" s="5" t="s">
-        <v>363</v>
+        <v>531</v>
       </c>
       <c r="K103" t="s">
         <v>371</v>
@@ -5472,7 +5610,7 @@
         <v>264</v>
       </c>
       <c r="J104" s="5" t="s">
-        <v>364</v>
+        <v>531</v>
       </c>
       <c r="K104" t="s">
         <v>368</v>
@@ -5507,7 +5645,7 @@
         <v>225</v>
       </c>
       <c r="J105" s="5" t="s">
-        <v>362</v>
+        <v>531</v>
       </c>
       <c r="K105" t="s">
         <v>370</v>

</xml_diff>